<commit_message>
12 season, 5 matchday
</commit_message>
<xml_diff>
--- a/output/bombs.xlsx
+++ b/output/bombs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -13,7 +13,7 @@
     <sheet name="4" sheetId="4" r:id="rId4"/>
     <sheet name="5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -701,8 +701,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -761,17 +761,22 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -809,7 +814,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -843,6 +848,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -877,9 +883,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1052,14 +1059,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1076,7 +1085,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>41</v>
       </c>
@@ -1096,7 +1105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42</v>
       </c>
@@ -1116,7 +1125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>9</v>
       </c>
@@ -1136,7 +1145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>55</v>
       </c>
@@ -1156,7 +1165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>27</v>
       </c>
@@ -1176,7 +1185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>61</v>
       </c>
@@ -1196,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>68</v>
       </c>
@@ -1216,7 +1225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>39</v>
       </c>
@@ -1236,7 +1245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>17</v>
       </c>
@@ -1256,7 +1265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>6</v>
       </c>
@@ -1276,7 +1285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>53</v>
       </c>
@@ -1296,7 +1305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>40</v>
       </c>
@@ -1316,7 +1325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>47</v>
       </c>
@@ -1330,13 +1339,13 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>64</v>
       </c>
@@ -1356,7 +1365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>57</v>
       </c>
@@ -1376,7 +1385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>35</v>
       </c>
@@ -1396,7 +1405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>65</v>
       </c>
@@ -1416,7 +1425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>80</v>
       </c>
@@ -1436,7 +1445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2</v>
       </c>
@@ -1456,7 +1465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>34</v>
       </c>
@@ -1476,7 +1485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -1496,7 +1505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>4</v>
       </c>
@@ -1516,7 +1525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44</v>
       </c>
@@ -1536,7 +1545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43</v>
       </c>
@@ -1556,7 +1565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>19</v>
       </c>
@@ -1576,7 +1585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>28</v>
       </c>
@@ -1596,7 +1605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>56</v>
       </c>
@@ -1616,7 +1625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>14</v>
       </c>
@@ -1636,7 +1645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>0</v>
       </c>
@@ -1656,7 +1665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>70</v>
       </c>
@@ -1676,7 +1685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>16</v>
       </c>
@@ -1696,7 +1705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>3</v>
       </c>
@@ -1710,13 +1719,13 @@
         <v>1</v>
       </c>
       <c r="E33">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>13</v>
       </c>
@@ -1736,7 +1745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>73</v>
       </c>
@@ -1756,7 +1765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>77</v>
       </c>
@@ -1776,7 +1785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>51</v>
       </c>
@@ -1796,7 +1805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>33</v>
       </c>
@@ -1816,7 +1825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>62</v>
       </c>
@@ -1836,7 +1845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>63</v>
       </c>
@@ -1856,7 +1865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>5</v>
       </c>
@@ -1876,7 +1885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>72</v>
       </c>
@@ -1902,14 +1911,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1926,7 +1935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>7</v>
       </c>
@@ -1946,7 +1955,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>16</v>
       </c>
@@ -1966,7 +1975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>61</v>
       </c>
@@ -1986,7 +1995,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>53</v>
       </c>
@@ -2006,7 +2015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>25</v>
       </c>
@@ -2026,7 +2035,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>10</v>
       </c>
@@ -2046,7 +2055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>11</v>
       </c>
@@ -2066,7 +2075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>72</v>
       </c>
@@ -2086,7 +2095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>55</v>
       </c>
@@ -2106,7 +2115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>77</v>
       </c>
@@ -2126,7 +2135,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>21</v>
       </c>
@@ -2146,7 +2155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2166,7 +2175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>63</v>
       </c>
@@ -2186,7 +2195,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>50</v>
       </c>
@@ -2206,7 +2215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>42</v>
       </c>
@@ -2226,7 +2235,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>19</v>
       </c>
@@ -2246,7 +2255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>30</v>
       </c>
@@ -2266,7 +2275,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>80</v>
       </c>
@@ -2286,7 +2295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>34</v>
       </c>
@@ -2306,7 +2315,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>40</v>
       </c>
@@ -2326,7 +2335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>68</v>
       </c>
@@ -2346,7 +2355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>62</v>
       </c>
@@ -2366,7 +2375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>36</v>
       </c>
@@ -2386,7 +2395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>74</v>
       </c>
@@ -2406,7 +2415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>28</v>
       </c>
@@ -2426,7 +2435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>75</v>
       </c>
@@ -2446,7 +2455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>70</v>
       </c>
@@ -2466,7 +2475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43</v>
       </c>
@@ -2486,7 +2495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>69</v>
       </c>
@@ -2506,7 +2515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45</v>
       </c>
@@ -2526,7 +2535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>51</v>
       </c>
@@ -2546,7 +2555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>9</v>
       </c>
@@ -2572,14 +2581,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2596,7 +2605,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>50</v>
       </c>
@@ -2616,7 +2625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>52</v>
       </c>
@@ -2636,7 +2645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>70</v>
       </c>
@@ -2656,7 +2665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>63</v>
       </c>
@@ -2676,7 +2685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -2696,7 +2705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>61</v>
       </c>
@@ -2716,7 +2725,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>79</v>
       </c>
@@ -2736,7 +2745,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>26</v>
       </c>
@@ -2756,7 +2765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>68</v>
       </c>
@@ -2776,7 +2785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>55</v>
       </c>
@@ -2796,7 +2805,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -2816,7 +2825,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>72</v>
       </c>
@@ -2836,7 +2845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>57</v>
       </c>
@@ -2856,7 +2865,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>16</v>
       </c>
@@ -2876,7 +2885,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>41</v>
       </c>
@@ -2896,7 +2905,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>31</v>
       </c>
@@ -2916,7 +2925,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>5</v>
       </c>
@@ -2936,7 +2945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>67</v>
       </c>
@@ -2956,7 +2965,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>13</v>
       </c>
@@ -2976,7 +2985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>40</v>
       </c>
@@ -2996,7 +3005,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>35</v>
       </c>
@@ -3016,7 +3025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>39</v>
       </c>
@@ -3036,7 +3045,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>75</v>
       </c>
@@ -3056,7 +3065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>66</v>
       </c>
@@ -3076,7 +3085,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>7</v>
       </c>
@@ -3096,7 +3105,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>42</v>
       </c>
@@ -3116,7 +3125,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>46</v>
       </c>
@@ -3136,7 +3145,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>78</v>
       </c>
@@ -3156,7 +3165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>10</v>
       </c>
@@ -3176,7 +3185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>76</v>
       </c>
@@ -3196,7 +3205,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>56</v>
       </c>
@@ -3216,7 +3225,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>20</v>
       </c>
@@ -3236,7 +3245,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>34</v>
       </c>
@@ -3256,7 +3265,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>73</v>
       </c>
@@ -3276,7 +3285,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>37</v>
       </c>
@@ -3296,7 +3305,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>65</v>
       </c>
@@ -3316,7 +3325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>25</v>
       </c>
@@ -3336,7 +3345,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>3</v>
       </c>
@@ -3362,14 +3371,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3386,7 +3395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>50</v>
       </c>
@@ -3406,7 +3415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>31</v>
       </c>
@@ -3426,7 +3435,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>65</v>
       </c>
@@ -3446,7 +3455,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -3466,7 +3475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>61</v>
       </c>
@@ -3486,7 +3495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>33</v>
       </c>
@@ -3506,7 +3515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>21</v>
       </c>
@@ -3526,7 +3535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>60</v>
       </c>
@@ -3546,7 +3555,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>59</v>
       </c>
@@ -3566,7 +3575,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>75</v>
       </c>
@@ -3586,7 +3595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>19</v>
       </c>
@@ -3606,7 +3615,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>72</v>
       </c>
@@ -3626,7 +3635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>62</v>
       </c>
@@ -3646,7 +3655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>77</v>
       </c>
@@ -3666,7 +3675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>35</v>
       </c>
@@ -3686,7 +3695,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>69</v>
       </c>
@@ -3706,7 +3715,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -3726,7 +3735,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>14</v>
       </c>
@@ -3746,7 +3755,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>4</v>
       </c>
@@ -3766,7 +3775,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -3786,7 +3795,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>24</v>
       </c>
@@ -3806,7 +3815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>7</v>
       </c>
@@ -3826,7 +3835,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>67</v>
       </c>
@@ -3846,7 +3855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>79</v>
       </c>
@@ -3866,7 +3875,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2</v>
       </c>
@@ -3886,7 +3895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>38</v>
       </c>
@@ -3906,7 +3915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>52</v>
       </c>
@@ -3926,7 +3935,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -3946,7 +3955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>36</v>
       </c>
@@ -3966,7 +3975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>46</v>
       </c>
@@ -3992,14 +4001,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4016,7 +4025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>14</v>
       </c>
@@ -4036,7 +4045,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>46</v>
       </c>
@@ -4056,7 +4065,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>63</v>
       </c>
@@ -4076,7 +4085,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>70</v>
       </c>
@@ -4096,7 +4105,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>15</v>
       </c>
@@ -4116,7 +4125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>78</v>
       </c>
@@ -4136,7 +4145,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>77</v>
       </c>
@@ -4156,7 +4165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>59</v>
       </c>
@@ -4176,7 +4185,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>79</v>
       </c>
@@ -4196,7 +4205,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>50</v>
       </c>
@@ -4216,7 +4225,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>60</v>
       </c>
@@ -4236,7 +4245,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>37</v>
       </c>
@@ -4256,7 +4265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>36</v>
       </c>
@@ -4276,7 +4285,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43</v>
       </c>
@@ -4296,7 +4305,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>68</v>
       </c>
@@ -4316,7 +4325,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>21</v>
       </c>
@@ -4336,7 +4345,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -4356,7 +4365,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>11</v>
       </c>
@@ -4376,7 +4385,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>72</v>
       </c>
@@ -4396,7 +4405,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>48</v>
       </c>
@@ -4416,7 +4425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>28</v>
       </c>
@@ -4436,7 +4445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>54</v>
       </c>
@@ -4456,7 +4465,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>65</v>
       </c>
@@ -4476,7 +4485,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>7</v>
       </c>
@@ -4496,7 +4505,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>75</v>
       </c>
@@ -4516,7 +4525,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>61</v>
       </c>
@@ -4536,7 +4545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>58</v>
       </c>
@@ -4556,7 +4565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>80</v>
       </c>
@@ -4576,7 +4585,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>0</v>
       </c>
@@ -4596,7 +4605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -4616,7 +4625,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>25</v>
       </c>
@@ -4636,7 +4645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>71</v>
       </c>
@@ -4656,7 +4665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
Updated 7 matchday, 12 season
</commit_message>
<xml_diff>
--- a/output/bombs.xlsx
+++ b/output/bombs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -12,13 +12,15 @@
     <sheet name="3" sheetId="3" r:id="rId3"/>
     <sheet name="4" sheetId="4" r:id="rId4"/>
     <sheet name="5" sheetId="5" r:id="rId5"/>
+    <sheet name="6" sheetId="6" r:id="rId6"/>
+    <sheet name="7" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="276">
   <si>
     <t>Scorer</t>
   </si>
@@ -696,13 +698,163 @@
   </si>
   <si>
     <t>арс</t>
+  </si>
+  <si>
+    <t>аллер</t>
+  </si>
+  <si>
+    <t>антони</t>
+  </si>
+  <si>
+    <t>артур</t>
+  </si>
+  <si>
+    <t>бакасетас</t>
+  </si>
+  <si>
+    <t>бебу</t>
+  </si>
+  <si>
+    <t>влахович</t>
+  </si>
+  <si>
+    <t>влашич</t>
+  </si>
+  <si>
+    <t>гийомено</t>
+  </si>
+  <si>
+    <t>гризман</t>
+  </si>
+  <si>
+    <t>де йонг</t>
+  </si>
+  <si>
+    <t>кабрал</t>
+  </si>
+  <si>
+    <t>дуа</t>
+  </si>
+  <si>
+    <t>классен</t>
+  </si>
+  <si>
+    <t>кокорин</t>
+  </si>
+  <si>
+    <t>ляказетт</t>
+  </si>
+  <si>
+    <t>маунт</t>
+  </si>
+  <si>
+    <t>моллен</t>
+  </si>
+  <si>
+    <t>нвакаэме</t>
+  </si>
+  <si>
+    <t>рэшфорд</t>
+  </si>
+  <si>
+    <t>фарду</t>
+  </si>
+  <si>
+    <t>базель</t>
+  </si>
+  <si>
+    <t>трабзонспор</t>
+  </si>
+  <si>
+    <t>хофенхайм</t>
+  </si>
+  <si>
+    <t>цска</t>
+  </si>
+  <si>
+    <t>санкт-галлен</t>
+  </si>
+  <si>
+    <t>ман юнайтед</t>
+  </si>
+  <si>
+    <t>боаду</t>
+  </si>
+  <si>
+    <t>броя</t>
+  </si>
+  <si>
+    <t>вольф</t>
+  </si>
+  <si>
+    <t>заболотный</t>
+  </si>
+  <si>
+    <t>ихеначо</t>
+  </si>
+  <si>
+    <t>копмейнерс</t>
+  </si>
+  <si>
+    <t>ларссон</t>
+  </si>
+  <si>
+    <t>мартинес</t>
+  </si>
+  <si>
+    <t>плеа</t>
+  </si>
+  <si>
+    <t>понсе</t>
+  </si>
+  <si>
+    <t>промес</t>
+  </si>
+  <si>
+    <t>санчес</t>
+  </si>
+  <si>
+    <t>сарджент</t>
+  </si>
+  <si>
+    <t>соу</t>
+  </si>
+  <si>
+    <t>феликс</t>
+  </si>
+  <si>
+    <t>хоффман</t>
+  </si>
+  <si>
+    <t>шик</t>
+  </si>
+  <si>
+    <t>аз</t>
+  </si>
+  <si>
+    <t>витесс</t>
+  </si>
+  <si>
+    <t>кельн</t>
+  </si>
+  <si>
+    <t>сочи</t>
+  </si>
+  <si>
+    <t>спартак</t>
+  </si>
+  <si>
+    <t>ростов</t>
+  </si>
+  <si>
+    <t>байер</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -761,22 +913,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -814,7 +961,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -848,7 +995,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -883,10 +1029,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1059,16 +1204,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1085,7 +1228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>41</v>
       </c>
@@ -1105,7 +1248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>42</v>
       </c>
@@ -1125,7 +1268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>9</v>
       </c>
@@ -1145,7 +1288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>55</v>
       </c>
@@ -1165,7 +1308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>27</v>
       </c>
@@ -1185,7 +1328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>61</v>
       </c>
@@ -1205,7 +1348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>68</v>
       </c>
@@ -1225,7 +1368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>39</v>
       </c>
@@ -1245,7 +1388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>17</v>
       </c>
@@ -1265,7 +1408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>6</v>
       </c>
@@ -1285,7 +1428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>53</v>
       </c>
@@ -1305,7 +1448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>40</v>
       </c>
@@ -1325,7 +1468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>47</v>
       </c>
@@ -1345,7 +1488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>64</v>
       </c>
@@ -1365,7 +1508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>57</v>
       </c>
@@ -1385,7 +1528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>35</v>
       </c>
@@ -1405,7 +1548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>65</v>
       </c>
@@ -1425,7 +1568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>80</v>
       </c>
@@ -1445,7 +1588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>2</v>
       </c>
@@ -1465,7 +1608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>34</v>
       </c>
@@ -1485,7 +1628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -1505,7 +1648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>4</v>
       </c>
@@ -1525,7 +1668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>44</v>
       </c>
@@ -1545,7 +1688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>43</v>
       </c>
@@ -1565,7 +1708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>19</v>
       </c>
@@ -1585,7 +1728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>28</v>
       </c>
@@ -1605,7 +1748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="1">
         <v>56</v>
       </c>
@@ -1625,7 +1768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>14</v>
       </c>
@@ -1645,7 +1788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="1">
         <v>0</v>
       </c>
@@ -1665,7 +1808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="1">
         <v>70</v>
       </c>
@@ -1685,7 +1828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="1">
         <v>16</v>
       </c>
@@ -1705,7 +1848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="1">
         <v>3</v>
       </c>
@@ -1725,7 +1868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="1">
         <v>13</v>
       </c>
@@ -1745,7 +1888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="1">
         <v>73</v>
       </c>
@@ -1765,7 +1908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="1">
         <v>77</v>
       </c>
@@ -1785,7 +1928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="1">
         <v>51</v>
       </c>
@@ -1805,7 +1948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="1">
         <v>33</v>
       </c>
@@ -1825,7 +1968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="1">
         <v>62</v>
       </c>
@@ -1845,7 +1988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" s="1">
         <v>63</v>
       </c>
@@ -1865,7 +2008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" s="1">
         <v>5</v>
       </c>
@@ -1885,7 +2028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="1">
         <v>72</v>
       </c>
@@ -1911,14 +2054,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1935,7 +2078,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>7</v>
       </c>
@@ -1955,7 +2098,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>16</v>
       </c>
@@ -1975,7 +2118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>61</v>
       </c>
@@ -1995,7 +2138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>53</v>
       </c>
@@ -2015,7 +2158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>25</v>
       </c>
@@ -2035,7 +2178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>10</v>
       </c>
@@ -2055,7 +2198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>11</v>
       </c>
@@ -2075,7 +2218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>72</v>
       </c>
@@ -2095,7 +2238,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>55</v>
       </c>
@@ -2115,7 +2258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>77</v>
       </c>
@@ -2135,7 +2278,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>21</v>
       </c>
@@ -2155,7 +2298,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2175,7 +2318,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>63</v>
       </c>
@@ -2195,7 +2338,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>50</v>
       </c>
@@ -2215,7 +2358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>42</v>
       </c>
@@ -2235,7 +2378,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>19</v>
       </c>
@@ -2255,7 +2398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>30</v>
       </c>
@@ -2275,7 +2418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>80</v>
       </c>
@@ -2295,7 +2438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>34</v>
       </c>
@@ -2315,7 +2458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>40</v>
       </c>
@@ -2335,7 +2478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>68</v>
       </c>
@@ -2355,7 +2498,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>62</v>
       </c>
@@ -2375,7 +2518,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>36</v>
       </c>
@@ -2395,7 +2538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>74</v>
       </c>
@@ -2415,7 +2558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>28</v>
       </c>
@@ -2435,7 +2578,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>75</v>
       </c>
@@ -2455,7 +2598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="1">
         <v>70</v>
       </c>
@@ -2475,7 +2618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>43</v>
       </c>
@@ -2495,7 +2638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="1">
         <v>69</v>
       </c>
@@ -2515,7 +2658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="1">
         <v>45</v>
       </c>
@@ -2535,7 +2678,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="1">
         <v>51</v>
       </c>
@@ -2555,7 +2698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="1">
         <v>9</v>
       </c>
@@ -2581,14 +2724,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2605,7 +2748,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>50</v>
       </c>
@@ -2625,7 +2768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>52</v>
       </c>
@@ -2645,7 +2788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>70</v>
       </c>
@@ -2665,7 +2808,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>63</v>
       </c>
@@ -2685,7 +2828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -2705,7 +2848,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>61</v>
       </c>
@@ -2725,7 +2868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>79</v>
       </c>
@@ -2745,7 +2888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>26</v>
       </c>
@@ -2765,7 +2908,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>68</v>
       </c>
@@ -2785,7 +2928,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>55</v>
       </c>
@@ -2805,7 +2948,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -2825,7 +2968,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>72</v>
       </c>
@@ -2845,7 +2988,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>57</v>
       </c>
@@ -2865,7 +3008,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>16</v>
       </c>
@@ -2885,7 +3028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>41</v>
       </c>
@@ -2905,7 +3048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>31</v>
       </c>
@@ -2925,7 +3068,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>5</v>
       </c>
@@ -2945,7 +3088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>67</v>
       </c>
@@ -2965,7 +3108,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>13</v>
       </c>
@@ -2985,7 +3128,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>40</v>
       </c>
@@ -3005,7 +3148,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>35</v>
       </c>
@@ -3025,7 +3168,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>39</v>
       </c>
@@ -3045,7 +3188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>75</v>
       </c>
@@ -3065,7 +3208,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>66</v>
       </c>
@@ -3085,7 +3228,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>7</v>
       </c>
@@ -3105,7 +3248,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>42</v>
       </c>
@@ -3125,7 +3268,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="1">
         <v>46</v>
       </c>
@@ -3145,7 +3288,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>78</v>
       </c>
@@ -3165,7 +3308,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="1">
         <v>10</v>
       </c>
@@ -3185,7 +3328,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="1">
         <v>76</v>
       </c>
@@ -3205,7 +3348,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="1">
         <v>56</v>
       </c>
@@ -3225,7 +3368,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="1">
         <v>20</v>
       </c>
@@ -3245,7 +3388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="1">
         <v>34</v>
       </c>
@@ -3265,7 +3408,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="1">
         <v>73</v>
       </c>
@@ -3285,7 +3428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="1">
         <v>37</v>
       </c>
@@ -3305,7 +3448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="1">
         <v>65</v>
       </c>
@@ -3325,7 +3468,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="1">
         <v>25</v>
       </c>
@@ -3345,7 +3488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="1">
         <v>3</v>
       </c>
@@ -3371,14 +3514,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3395,7 +3538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>50</v>
       </c>
@@ -3415,7 +3558,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>31</v>
       </c>
@@ -3435,7 +3578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>65</v>
       </c>
@@ -3455,7 +3598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -3475,7 +3618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>61</v>
       </c>
@@ -3495,7 +3638,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>33</v>
       </c>
@@ -3515,7 +3658,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>21</v>
       </c>
@@ -3535,7 +3678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>60</v>
       </c>
@@ -3555,7 +3698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>59</v>
       </c>
@@ -3575,7 +3718,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>75</v>
       </c>
@@ -3595,7 +3738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>19</v>
       </c>
@@ -3615,7 +3758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>72</v>
       </c>
@@ -3635,7 +3778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>62</v>
       </c>
@@ -3655,7 +3798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>77</v>
       </c>
@@ -3675,7 +3818,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>35</v>
       </c>
@@ -3695,7 +3838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>69</v>
       </c>
@@ -3715,7 +3858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -3735,7 +3878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>14</v>
       </c>
@@ -3755,7 +3898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>4</v>
       </c>
@@ -3775,7 +3918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -3795,7 +3938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>24</v>
       </c>
@@ -3815,7 +3958,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>7</v>
       </c>
@@ -3835,7 +3978,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>67</v>
       </c>
@@ -3855,7 +3998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>79</v>
       </c>
@@ -3875,7 +4018,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>2</v>
       </c>
@@ -3895,7 +4038,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>38</v>
       </c>
@@ -3915,7 +4058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="1">
         <v>52</v>
       </c>
@@ -3935,7 +4078,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -3955,7 +4098,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="1">
         <v>36</v>
       </c>
@@ -3975,7 +4118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="1">
         <v>46</v>
       </c>
@@ -4001,14 +4144,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4025,7 +4168,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>14</v>
       </c>
@@ -4045,7 +4188,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>46</v>
       </c>
@@ -4065,7 +4208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>63</v>
       </c>
@@ -4085,7 +4228,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>70</v>
       </c>
@@ -4105,7 +4248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>15</v>
       </c>
@@ -4125,7 +4268,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>78</v>
       </c>
@@ -4145,7 +4288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>77</v>
       </c>
@@ -4165,7 +4308,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>59</v>
       </c>
@@ -4185,7 +4328,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>79</v>
       </c>
@@ -4205,7 +4348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>50</v>
       </c>
@@ -4225,7 +4368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>60</v>
       </c>
@@ -4245,7 +4388,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>37</v>
       </c>
@@ -4265,7 +4408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>36</v>
       </c>
@@ -4285,7 +4428,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>43</v>
       </c>
@@ -4305,7 +4448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>68</v>
       </c>
@@ -4325,7 +4468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>21</v>
       </c>
@@ -4345,7 +4488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -4365,7 +4508,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="1">
         <v>11</v>
       </c>
@@ -4385,7 +4528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="1">
         <v>72</v>
       </c>
@@ -4405,7 +4548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="1">
         <v>48</v>
       </c>
@@ -4425,7 +4568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="1">
         <v>28</v>
       </c>
@@ -4445,7 +4588,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="1">
         <v>54</v>
       </c>
@@ -4465,7 +4608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="1">
         <v>65</v>
       </c>
@@ -4485,7 +4628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="1">
         <v>7</v>
       </c>
@@ -4505,7 +4648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="1">
         <v>75</v>
       </c>
@@ -4525,7 +4668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="1">
         <v>61</v>
       </c>
@@ -4545,7 +4688,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="1">
         <v>58</v>
       </c>
@@ -4565,7 +4708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="1">
         <v>80</v>
       </c>
@@ -4585,7 +4728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="1">
         <v>0</v>
       </c>
@@ -4605,7 +4748,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -4625,7 +4768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="1">
         <v>25</v>
       </c>
@@ -4645,7 +4788,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="1">
         <v>71</v>
       </c>
@@ -4665,7 +4808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="1">
         <v>52</v>
       </c>
@@ -4683,6 +4826,1426 @@
       </c>
       <c r="F34">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C4" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C7" t="s">
+        <v>248</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" t="s">
+        <v>147</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>231</v>
+      </c>
+      <c r="C11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>232</v>
+      </c>
+      <c r="C12" t="s">
+        <v>249</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>233</v>
+      </c>
+      <c r="C13" t="s">
+        <v>250</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>234</v>
+      </c>
+      <c r="C14" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>235</v>
+      </c>
+      <c r="C15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>59</v>
+      </c>
+      <c r="B17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>203</v>
+      </c>
+      <c r="C18" t="s">
+        <v>220</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>163</v>
+      </c>
+      <c r="C19" t="s">
+        <v>186</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>236</v>
+      </c>
+      <c r="C20" t="s">
+        <v>246</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1">
+        <v>65</v>
+      </c>
+      <c r="B21" t="s">
+        <v>237</v>
+      </c>
+      <c r="C21" t="s">
+        <v>250</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
+        <v>238</v>
+      </c>
+      <c r="C22" t="s">
+        <v>155</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>239</v>
+      </c>
+      <c r="C23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1">
+        <v>31</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1">
+        <v>67</v>
+      </c>
+      <c r="B25" t="s">
+        <v>240</v>
+      </c>
+      <c r="C25" t="s">
+        <v>153</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" t="s">
+        <v>147</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1">
+        <v>41</v>
+      </c>
+      <c r="B27" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" t="s">
+        <v>149</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>241</v>
+      </c>
+      <c r="C28" t="s">
+        <v>220</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1">
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C29" t="s">
+        <v>148</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="F29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>242</v>
+      </c>
+      <c r="C30" t="s">
+        <v>221</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1">
+        <v>55</v>
+      </c>
+      <c r="B31" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" t="s">
+        <v>147</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1">
+        <v>71</v>
+      </c>
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="1">
+        <v>17</v>
+      </c>
+      <c r="B33" t="s">
+        <v>243</v>
+      </c>
+      <c r="C33" t="s">
+        <v>247</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="1">
+        <v>62</v>
+      </c>
+      <c r="B34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" t="s">
+        <v>153</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="1">
+        <v>60</v>
+      </c>
+      <c r="B35" t="s">
+        <v>244</v>
+      </c>
+      <c r="C35" t="s">
+        <v>149</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="1">
+        <v>72</v>
+      </c>
+      <c r="B36" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" t="s">
+        <v>155</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="1">
+        <v>68</v>
+      </c>
+      <c r="B37" t="s">
+        <v>245</v>
+      </c>
+      <c r="C37" t="s">
+        <v>186</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="1">
+        <v>27</v>
+      </c>
+      <c r="B38" t="s">
+        <v>134</v>
+      </c>
+      <c r="C38" t="s">
+        <v>251</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="1">
+        <v>9</v>
+      </c>
+      <c r="B39" t="s">
+        <v>217</v>
+      </c>
+      <c r="C39" t="s">
+        <v>155</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="1">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>140</v>
+      </c>
+      <c r="C40" t="s">
+        <v>150</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>252</v>
+      </c>
+      <c r="C3" t="s">
+        <v>269</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>253</v>
+      </c>
+      <c r="C4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>254</v>
+      </c>
+      <c r="C7" t="s">
+        <v>271</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>71</v>
+      </c>
+      <c r="B8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>255</v>
+      </c>
+      <c r="C9" t="s">
+        <v>272</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>256</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>257</v>
+      </c>
+      <c r="C11" t="s">
+        <v>269</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s">
+        <v>258</v>
+      </c>
+      <c r="C13" t="s">
+        <v>273</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C14" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>15</v>
+      </c>
+      <c r="F14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>259</v>
+      </c>
+      <c r="C15" t="s">
+        <v>190</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
+        <v>171</v>
+      </c>
+      <c r="C17" t="s">
+        <v>191</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>260</v>
+      </c>
+      <c r="C18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>64</v>
+      </c>
+      <c r="B19" t="s">
+        <v>261</v>
+      </c>
+      <c r="C19" t="s">
+        <v>273</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>262</v>
+      </c>
+      <c r="C20" t="s">
+        <v>273</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s">
+        <v>263</v>
+      </c>
+      <c r="C21" t="s">
+        <v>190</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>264</v>
+      </c>
+      <c r="C22" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>265</v>
+      </c>
+      <c r="C23" t="s">
+        <v>274</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>215</v>
+      </c>
+      <c r="C24" t="s">
+        <v>224</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>6</v>
+      </c>
+      <c r="F24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>207</v>
+      </c>
+      <c r="C25" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1">
+        <v>69</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>266</v>
+      </c>
+      <c r="C28" t="s">
+        <v>224</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1">
+        <v>37</v>
+      </c>
+      <c r="B29" t="s">
+        <v>267</v>
+      </c>
+      <c r="C29" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1">
+        <v>51</v>
+      </c>
+      <c r="B30" t="s">
+        <v>268</v>
+      </c>
+      <c r="C30" t="s">
+        <v>275</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
12 season, 7-8 Matchdays
</commit_message>
<xml_diff>
--- a/output/bombs.xlsx
+++ b/output/bombs.xlsx
@@ -14,13 +14,15 @@
     <sheet name="5" sheetId="5" r:id="rId5"/>
     <sheet name="6" sheetId="6" r:id="rId6"/>
     <sheet name="7" sheetId="7" r:id="rId7"/>
+    <sheet name="8" sheetId="8" r:id="rId8"/>
+    <sheet name="9" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="314">
   <si>
     <t>Scorer</t>
   </si>
@@ -848,6 +850,120 @@
   </si>
   <si>
     <t>байер</t>
+  </si>
+  <si>
+    <t>алькасер</t>
+  </si>
+  <si>
+    <t>бэйл</t>
+  </si>
+  <si>
+    <t>винисиус</t>
+  </si>
+  <si>
+    <t>кент</t>
+  </si>
+  <si>
+    <t>молина</t>
+  </si>
+  <si>
+    <t>морелос</t>
+  </si>
+  <si>
+    <t>станчу</t>
+  </si>
+  <si>
+    <t>вильярреал</t>
+  </si>
+  <si>
+    <t>барса</t>
+  </si>
+  <si>
+    <t>рейнджерс</t>
+  </si>
+  <si>
+    <t>славия</t>
+  </si>
+  <si>
+    <t>аспас</t>
+  </si>
+  <si>
+    <t>бейл</t>
+  </si>
+  <si>
+    <t>бен-йеддер</t>
+  </si>
+  <si>
+    <t>буяльский</t>
+  </si>
+  <si>
+    <t>ван де стрек</t>
+  </si>
+  <si>
+    <t>гладкий</t>
+  </si>
+  <si>
+    <t>дестро</t>
+  </si>
+  <si>
+    <t>захеди</t>
+  </si>
+  <si>
+    <t>ингс</t>
+  </si>
+  <si>
+    <t>инсинье</t>
+  </si>
+  <si>
+    <t>кессье</t>
+  </si>
+  <si>
+    <t>кулибали</t>
+  </si>
+  <si>
+    <t>леау</t>
+  </si>
+  <si>
+    <t>махи</t>
+  </si>
+  <si>
+    <t>мина</t>
+  </si>
+  <si>
+    <t>опенда</t>
+  </si>
+  <si>
+    <t>соболев</t>
+  </si>
+  <si>
+    <t>фолланд</t>
+  </si>
+  <si>
+    <t>фомин</t>
+  </si>
+  <si>
+    <t>эдегор</t>
+  </si>
+  <si>
+    <t>эндо</t>
+  </si>
+  <si>
+    <t>сельта</t>
+  </si>
+  <si>
+    <t>монако</t>
+  </si>
+  <si>
+    <t>утрехт</t>
+  </si>
+  <si>
+    <t>заря</t>
+  </si>
+  <si>
+    <t>дженоа</t>
+  </si>
+  <si>
+    <t>динамо москва</t>
   </si>
 </sst>
 </file>
@@ -6251,4 +6367,1284 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>55</v>
+      </c>
+      <c r="B2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C2" t="s">
+        <v>283</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C4" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>278</v>
+      </c>
+      <c r="C5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s">
+        <v>234</v>
+      </c>
+      <c r="C6" t="s">
+        <v>284</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" t="s">
+        <v>194</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>75</v>
+      </c>
+      <c r="B8" t="s">
+        <v>279</v>
+      </c>
+      <c r="C8" t="s">
+        <v>285</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>65</v>
+      </c>
+      <c r="B13" t="s">
+        <v>280</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>281</v>
+      </c>
+      <c r="C15" t="s">
+        <v>285</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>170</v>
+      </c>
+      <c r="C16" t="s">
+        <v>283</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>173</v>
+      </c>
+      <c r="C17" t="s">
+        <v>194</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>12</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
+        <v>244</v>
+      </c>
+      <c r="C19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1">
+        <v>74</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21" t="s">
+        <v>194</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
+        <v>282</v>
+      </c>
+      <c r="C22" t="s">
+        <v>286</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1">
+        <v>66</v>
+      </c>
+      <c r="B23" t="s">
+        <v>134</v>
+      </c>
+      <c r="C23" t="s">
+        <v>149</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" t="s">
+        <v>154</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>13</v>
+      </c>
+      <c r="F24">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C4" t="s">
+        <v>309</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>253</v>
+      </c>
+      <c r="C6" t="s">
+        <v>270</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>73</v>
+      </c>
+      <c r="B8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>291</v>
+      </c>
+      <c r="C9" t="s">
+        <v>310</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
+        <v>292</v>
+      </c>
+      <c r="C10" t="s">
+        <v>311</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>293</v>
+      </c>
+      <c r="C12" t="s">
+        <v>312</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>294</v>
+      </c>
+      <c r="C13" t="s">
+        <v>311</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>163</v>
+      </c>
+      <c r="C14" t="s">
+        <v>186</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>295</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>296</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>165</v>
+      </c>
+      <c r="C18" t="s">
+        <v>194</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>9</v>
+      </c>
+      <c r="F18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>297</v>
+      </c>
+      <c r="C19" t="s">
+        <v>186</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1">
+        <v>67</v>
+      </c>
+      <c r="B21" t="s">
+        <v>298</v>
+      </c>
+      <c r="C21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>258</v>
+      </c>
+      <c r="C22" t="s">
+        <v>273</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>299</v>
+      </c>
+      <c r="C23" t="s">
+        <v>186</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>210</v>
+      </c>
+      <c r="C24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
+        <v>240</v>
+      </c>
+      <c r="C25" t="s">
+        <v>153</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1">
+        <v>53</v>
+      </c>
+      <c r="B26" t="s">
+        <v>300</v>
+      </c>
+      <c r="C26" t="s">
+        <v>310</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1">
+        <v>33</v>
+      </c>
+      <c r="B27" t="s">
+        <v>301</v>
+      </c>
+      <c r="C27" t="s">
+        <v>308</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1">
+        <v>66</v>
+      </c>
+      <c r="B29" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" t="s">
+        <v>153</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>302</v>
+      </c>
+      <c r="C30" t="s">
+        <v>270</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1">
+        <v>16</v>
+      </c>
+      <c r="B31" t="s">
+        <v>261</v>
+      </c>
+      <c r="C31" t="s">
+        <v>273</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>262</v>
+      </c>
+      <c r="C32" t="s">
+        <v>273</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="1">
+        <v>10</v>
+      </c>
+      <c r="B33" t="s">
+        <v>303</v>
+      </c>
+      <c r="C33" t="s">
+        <v>273</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="1">
+        <v>63</v>
+      </c>
+      <c r="B34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="1">
+        <v>61</v>
+      </c>
+      <c r="B35" t="s">
+        <v>304</v>
+      </c>
+      <c r="C35" t="s">
+        <v>309</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="1">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>305</v>
+      </c>
+      <c r="C36" t="s">
+        <v>313</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="1">
+        <v>65</v>
+      </c>
+      <c r="B37" t="s">
+        <v>137</v>
+      </c>
+      <c r="C37" t="s">
+        <v>145</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>6</v>
+      </c>
+      <c r="F37">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="1">
+        <v>76</v>
+      </c>
+      <c r="B38" t="s">
+        <v>306</v>
+      </c>
+      <c r="C38" t="s">
+        <v>153</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="1">
+        <v>50</v>
+      </c>
+      <c r="B39" t="s">
+        <v>307</v>
+      </c>
+      <c r="C39" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Season 12, Matchday 11
</commit_message>
<xml_diff>
--- a/output/bombs.xlsx
+++ b/output/bombs.xlsx
@@ -16,13 +16,15 @@
     <sheet name="7" sheetId="7" r:id="rId7"/>
     <sheet name="8" sheetId="8" r:id="rId8"/>
     <sheet name="9" sheetId="9" r:id="rId9"/>
+    <sheet name="10" sheetId="10" r:id="rId10"/>
+    <sheet name="11" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="349">
   <si>
     <t>Scorer</t>
   </si>
@@ -964,6 +966,111 @@
   </si>
   <si>
     <t>динамо москва</t>
+  </si>
+  <si>
+    <t>агуеро</t>
+  </si>
+  <si>
+    <t>гнабри</t>
+  </si>
+  <si>
+    <t>госенс</t>
+  </si>
+  <si>
+    <t>де брюйне</t>
+  </si>
+  <si>
+    <t>карраско</t>
+  </si>
+  <si>
+    <t>нерес</t>
+  </si>
+  <si>
+    <t>нсаме</t>
+  </si>
+  <si>
+    <t>эйкрейм</t>
+  </si>
+  <si>
+    <t>янг бойз</t>
+  </si>
+  <si>
+    <t>мольде</t>
+  </si>
+  <si>
+    <t>абубакар</t>
+  </si>
+  <si>
+    <t>ауар</t>
+  </si>
+  <si>
+    <t>бэмфорд</t>
+  </si>
+  <si>
+    <t>депай</t>
+  </si>
+  <si>
+    <t>долберг</t>
+  </si>
+  <si>
+    <t>корне</t>
+  </si>
+  <si>
+    <t>крессвелл</t>
+  </si>
+  <si>
+    <t>кюизанс</t>
+  </si>
+  <si>
+    <t>ларин</t>
+  </si>
+  <si>
+    <t>лингард</t>
+  </si>
+  <si>
+    <t>милик</t>
+  </si>
+  <si>
+    <t>осимхен</t>
+  </si>
+  <si>
+    <t>пайет</t>
+  </si>
+  <si>
+    <t>рафинья</t>
+  </si>
+  <si>
+    <t>соучек</t>
+  </si>
+  <si>
+    <t>эдуард</t>
+  </si>
+  <si>
+    <t>бешикташ</t>
+  </si>
+  <si>
+    <t>лион</t>
+  </si>
+  <si>
+    <t>аз алкмар</t>
+  </si>
+  <si>
+    <t>лидс</t>
+  </si>
+  <si>
+    <t>ницца</t>
+  </si>
+  <si>
+    <t>вэст хэм</t>
+  </si>
+  <si>
+    <t>вест хэм</t>
+  </si>
+  <si>
+    <t>рейджерс</t>
+  </si>
+  <si>
+    <t>селтик</t>
   </si>
 </sst>
 </file>
@@ -2169,6 +2276,1306 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>315</v>
+      </c>
+      <c r="C5" t="s">
+        <v>223</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>316</v>
+      </c>
+      <c r="C6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>317</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>205</v>
+      </c>
+      <c r="C11" t="s">
+        <v>222</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>318</v>
+      </c>
+      <c r="C12" t="s">
+        <v>224</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>71</v>
+      </c>
+      <c r="B13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13" t="s">
+        <v>194</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>206</v>
+      </c>
+      <c r="C14" t="s">
+        <v>223</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>208</v>
+      </c>
+      <c r="C15" t="s">
+        <v>223</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>18</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>240</v>
+      </c>
+      <c r="C16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>55</v>
+      </c>
+      <c r="B18" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>281</v>
+      </c>
+      <c r="C19" t="s">
+        <v>285</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s">
+        <v>170</v>
+      </c>
+      <c r="C20" t="s">
+        <v>283</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1">
+        <v>64</v>
+      </c>
+      <c r="B21" t="s">
+        <v>171</v>
+      </c>
+      <c r="C21" t="s">
+        <v>191</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s">
+        <v>319</v>
+      </c>
+      <c r="C22" t="s">
+        <v>155</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1">
+        <v>76</v>
+      </c>
+      <c r="B23" t="s">
+        <v>320</v>
+      </c>
+      <c r="C23" t="s">
+        <v>322</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1">
+        <v>63</v>
+      </c>
+      <c r="B25" t="s">
+        <v>213</v>
+      </c>
+      <c r="C25" t="s">
+        <v>283</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>177</v>
+      </c>
+      <c r="C26" t="s">
+        <v>191</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>178</v>
+      </c>
+      <c r="C27" t="s">
+        <v>194</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1">
+        <v>70</v>
+      </c>
+      <c r="B29" t="s">
+        <v>215</v>
+      </c>
+      <c r="C29" t="s">
+        <v>224</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>133</v>
+      </c>
+      <c r="C30" t="s">
+        <v>155</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1">
+        <v>11</v>
+      </c>
+      <c r="B31" t="s">
+        <v>134</v>
+      </c>
+      <c r="C31" t="s">
+        <v>149</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="1">
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
+        <v>321</v>
+      </c>
+      <c r="C32" t="s">
+        <v>323</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="1">
+        <v>67</v>
+      </c>
+      <c r="B33" t="s">
+        <v>182</v>
+      </c>
+      <c r="C33" t="s">
+        <v>186</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" t="s">
+        <v>340</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C4" t="s">
+        <v>342</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>326</v>
+      </c>
+      <c r="C5" t="s">
+        <v>343</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>327</v>
+      </c>
+      <c r="C6" t="s">
+        <v>341</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>328</v>
+      </c>
+      <c r="C7" t="s">
+        <v>344</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="1">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>296</v>
+      </c>
+      <c r="C9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>297</v>
+      </c>
+      <c r="C10" t="s">
+        <v>186</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="1">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
+        <v>257</v>
+      </c>
+      <c r="C11" t="s">
+        <v>342</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="1">
+        <v>76</v>
+      </c>
+      <c r="B12" t="s">
+        <v>329</v>
+      </c>
+      <c r="C12" t="s">
+        <v>341</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="1">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>330</v>
+      </c>
+      <c r="C13" t="s">
+        <v>345</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1">
+        <v>68</v>
+      </c>
+      <c r="B14" t="s">
+        <v>331</v>
+      </c>
+      <c r="C14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="1">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>332</v>
+      </c>
+      <c r="C15" t="s">
+        <v>340</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="1">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>333</v>
+      </c>
+      <c r="C16" t="s">
+        <v>346</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="1">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>240</v>
+      </c>
+      <c r="C17" t="s">
+        <v>153</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="1">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>211</v>
+      </c>
+      <c r="C18" t="s">
+        <v>221</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="1">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" t="s">
+        <v>151</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>12</v>
+      </c>
+      <c r="F19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="1">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>169</v>
+      </c>
+      <c r="C20" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>334</v>
+      </c>
+      <c r="C21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>281</v>
+      </c>
+      <c r="C22" t="s">
+        <v>347</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="1">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" t="s">
+        <v>151</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="1">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>335</v>
+      </c>
+      <c r="C24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="1">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
+        <v>336</v>
+      </c>
+      <c r="C25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="1">
+        <v>63</v>
+      </c>
+      <c r="B26" t="s">
+        <v>337</v>
+      </c>
+      <c r="C26" t="s">
+        <v>343</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="1">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" t="s">
+        <v>152</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1">
+        <v>30</v>
+      </c>
+      <c r="B28" t="s">
+        <v>338</v>
+      </c>
+      <c r="C28" t="s">
+        <v>346</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="1">
+        <v>42</v>
+      </c>
+      <c r="B30" t="s">
+        <v>306</v>
+      </c>
+      <c r="C30" t="s">
+        <v>153</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="1">
+        <v>41</v>
+      </c>
+      <c r="B31" t="s">
+        <v>339</v>
+      </c>
+      <c r="C31" t="s">
+        <v>348</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F33"/>

</xml_diff>

<commit_message>
Season 14, bombs 11
</commit_message>
<xml_diff>
--- a/output/bombs.xlsx
+++ b/output/bombs.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\euroleague\output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448582C2-469B-434F-A0EC-940DB731CAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="10836" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -17,13 +23,14 @@
     <sheet name="8" sheetId="8" r:id="rId8"/>
     <sheet name="9" sheetId="9" r:id="rId9"/>
     <sheet name="10" sheetId="10" r:id="rId10"/>
+    <sheet name="11" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="292">
   <si>
     <t>Team</t>
   </si>
@@ -830,13 +837,82 @@
   </si>
   <si>
     <t>базель</t>
+  </si>
+  <si>
+    <t>аларио</t>
+  </si>
+  <si>
+    <t>ассомбалонга</t>
+  </si>
+  <si>
+    <t>балотелли</t>
+  </si>
+  <si>
+    <t>бла</t>
+  </si>
+  <si>
+    <t>винд</t>
+  </si>
+  <si>
+    <t>зайц</t>
+  </si>
+  <si>
+    <t>изидор</t>
+  </si>
+  <si>
+    <t>коло-муани</t>
+  </si>
+  <si>
+    <t>ляказетт</t>
+  </si>
+  <si>
+    <t>озил</t>
+  </si>
+  <si>
+    <t>сака</t>
+  </si>
+  <si>
+    <t>смит-роу</t>
+  </si>
+  <si>
+    <t>ундер</t>
+  </si>
+  <si>
+    <t>уткин</t>
+  </si>
+  <si>
+    <t>чикаллеши</t>
+  </si>
+  <si>
+    <t>эль-хадди</t>
+  </si>
+  <si>
+    <t>адана</t>
+  </si>
+  <si>
+    <t>адана демирспор</t>
+  </si>
+  <si>
+    <t>нант</t>
+  </si>
+  <si>
+    <t>вольфсбург</t>
+  </si>
+  <si>
+    <t>арсенал</t>
+  </si>
+  <si>
+    <t>ахмат</t>
+  </si>
+  <si>
+    <t>коньяспор</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -895,17 +971,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -943,9 +1027,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -977,9 +1061,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1011,9 +1113,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1186,14 +1306,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1210,7 +1332,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1227,7 +1349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1244,7 +1366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1261,7 +1383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1278,7 +1400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1295,7 +1417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1312,7 +1434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1329,7 +1451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1346,7 +1468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -1363,7 +1485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -1380,7 +1502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1397,7 +1519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1414,7 +1536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -1431,7 +1553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -1448,7 +1570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -1465,7 +1587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1482,7 +1604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -1499,7 +1621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -1516,7 +1638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -1533,7 +1655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>24</v>
       </c>
@@ -1550,7 +1672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1567,7 +1689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>26</v>
       </c>
@@ -1584,7 +1706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>27</v>
       </c>
@@ -1601,7 +1723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -1618,7 +1740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>29</v>
       </c>
@@ -1635,7 +1757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>30</v>
       </c>
@@ -1658,14 +1780,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1682,7 +1804,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>151</v>
       </c>
@@ -1699,7 +1821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>249</v>
       </c>
@@ -1716,7 +1838,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>250</v>
       </c>
@@ -1733,7 +1855,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>251</v>
       </c>
@@ -1750,7 +1872,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
@@ -1767,7 +1889,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>55</v>
       </c>
@@ -1784,7 +1906,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>252</v>
       </c>
@@ -1801,7 +1923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>253</v>
       </c>
@@ -1818,7 +1940,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>254</v>
       </c>
@@ -1835,7 +1957,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>255</v>
       </c>
@@ -1852,7 +1974,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>115</v>
       </c>
@@ -1869,7 +1991,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1886,7 +2008,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -1903,7 +2025,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>256</v>
       </c>
@@ -1920,7 +2042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>257</v>
       </c>
@@ -1937,7 +2059,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>117</v>
       </c>
@@ -1954,7 +2076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>258</v>
       </c>
@@ -1971,7 +2093,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>148</v>
       </c>
@@ -1988,7 +2110,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>259</v>
       </c>
@@ -2005,7 +2127,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>260</v>
       </c>
@@ -2022,7 +2144,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>261</v>
       </c>
@@ -2039,7 +2161,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>262</v>
       </c>
@@ -2056,7 +2178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>263</v>
       </c>
@@ -2073,7 +2195,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -2090,7 +2212,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>67</v>
       </c>
@@ -2105,6 +2227,531 @@
       </c>
       <c r="E26">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:E30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B4" t="s">
+        <v>285</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B7" t="s">
+        <v>287</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B8" t="s">
+        <v>288</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B14" t="s">
+        <v>247</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B16" t="s">
+        <v>287</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" t="s">
+        <v>184</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B18" t="s">
+        <v>289</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B19" t="s">
+        <v>213</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B22" t="s">
+        <v>186</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B23" t="s">
+        <v>289</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B24" t="s">
+        <v>289</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B25" t="s">
+        <v>214</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B26" t="s">
+        <v>213</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B27" t="s">
+        <v>290</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B28" t="s">
+        <v>291</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B29" t="s">
+        <v>186</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2113,14 +2760,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2137,7 +2784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
@@ -2154,7 +2801,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
@@ -2171,7 +2818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>48</v>
       </c>
@@ -2188,7 +2835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -2205,7 +2852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
@@ -2222,7 +2869,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
@@ -2239,7 +2886,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>52</v>
       </c>
@@ -2256,7 +2903,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>53</v>
       </c>
@@ -2273,7 +2920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
@@ -2290,7 +2937,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>55</v>
       </c>
@@ -2307,7 +2954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>56</v>
       </c>
@@ -2324,7 +2971,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -2341,7 +2988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>57</v>
       </c>
@@ -2358,7 +3005,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>58</v>
       </c>
@@ -2375,7 +3022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>59</v>
       </c>
@@ -2392,7 +3039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -2409,7 +3056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>60</v>
       </c>
@@ -2426,7 +3073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>61</v>
       </c>
@@ -2443,7 +3090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>62</v>
       </c>
@@ -2460,7 +3107,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>63</v>
       </c>
@@ -2477,7 +3124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>64</v>
       </c>
@@ -2494,7 +3141,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>65</v>
       </c>
@@ -2511,7 +3158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>66</v>
       </c>
@@ -2528,7 +3175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -2545,7 +3192,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>67</v>
       </c>
@@ -2562,7 +3209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>68</v>
       </c>
@@ -2585,14 +3232,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2609,7 +3256,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>83</v>
       </c>
@@ -2626,7 +3273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -2643,7 +3290,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>84</v>
       </c>
@@ -2660,7 +3307,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>53</v>
       </c>
@@ -2677,7 +3324,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>85</v>
       </c>
@@ -2694,7 +3341,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>86</v>
       </c>
@@ -2711,7 +3358,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>87</v>
       </c>
@@ -2728,7 +3375,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -2745,7 +3392,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -2762,7 +3409,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>88</v>
       </c>
@@ -2779,7 +3426,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>89</v>
       </c>
@@ -2796,7 +3443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>90</v>
       </c>
@@ -2813,7 +3460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -2830,7 +3477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -2847,7 +3494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>91</v>
       </c>
@@ -2864,7 +3511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>92</v>
       </c>
@@ -2881,7 +3528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>93</v>
       </c>
@@ -2898,7 +3545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>94</v>
       </c>
@@ -2915,7 +3562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>95</v>
       </c>
@@ -2932,7 +3579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>96</v>
       </c>
@@ -2949,7 +3596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>97</v>
       </c>
@@ -2966,7 +3613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>98</v>
       </c>
@@ -2983,7 +3630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>99</v>
       </c>
@@ -3000,7 +3647,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>100</v>
       </c>
@@ -3017,7 +3664,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>65</v>
       </c>
@@ -3034,7 +3681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>63</v>
       </c>
@@ -3051,7 +3698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>101</v>
       </c>
@@ -3068,7 +3715,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>102</v>
       </c>
@@ -3091,14 +3738,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -3115,7 +3762,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>112</v>
       </c>
@@ -3132,7 +3779,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>113</v>
       </c>
@@ -3149,7 +3796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>54</v>
       </c>
@@ -3166,7 +3813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>114</v>
       </c>
@@ -3183,7 +3830,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>115</v>
       </c>
@@ -3200,7 +3847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -3217,7 +3864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -3234,7 +3881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>59</v>
       </c>
@@ -3251,7 +3898,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>116</v>
       </c>
@@ -3268,7 +3915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>117</v>
       </c>
@@ -3285,7 +3932,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>118</v>
       </c>
@@ -3302,7 +3949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>119</v>
       </c>
@@ -3319,7 +3966,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -3336,7 +3983,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>120</v>
       </c>
@@ -3353,7 +4000,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>121</v>
       </c>
@@ -3370,7 +4017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>64</v>
       </c>
@@ -3387,7 +4034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>122</v>
       </c>
@@ -3404,7 +4051,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>123</v>
       </c>
@@ -3421,7 +4068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>124</v>
       </c>
@@ -3438,7 +4085,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>125</v>
       </c>
@@ -3455,7 +4102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>30</v>
       </c>
@@ -3472,7 +4119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>126</v>
       </c>
@@ -3495,14 +4142,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -3519,7 +4166,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>55</v>
       </c>
@@ -3536,7 +4183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>134</v>
       </c>
@@ -3553,7 +4200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>135</v>
       </c>
@@ -3570,7 +4217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>136</v>
       </c>
@@ -3587,7 +4234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>137</v>
       </c>
@@ -3604,7 +4251,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>138</v>
       </c>
@@ -3621,7 +4268,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>139</v>
       </c>
@@ -3638,7 +4285,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>140</v>
       </c>
@@ -3655,7 +4302,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>141</v>
       </c>
@@ -3672,7 +4319,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>142</v>
       </c>
@@ -3689,7 +4336,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -3706,7 +4353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>95</v>
       </c>
@@ -3723,7 +4370,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>143</v>
       </c>
@@ -3740,7 +4387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>144</v>
       </c>
@@ -3757,7 +4404,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>145</v>
       </c>
@@ -3774,7 +4421,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>146</v>
       </c>
@@ -3791,7 +4438,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>147</v>
       </c>
@@ -3808,7 +4455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>148</v>
       </c>
@@ -3825,7 +4472,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>149</v>
       </c>
@@ -3842,7 +4489,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>150</v>
       </c>
@@ -3859,7 +4506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>65</v>
       </c>
@@ -3876,7 +4523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>151</v>
       </c>
@@ -3893,7 +4540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -3916,14 +4563,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -3940,7 +4587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>159</v>
       </c>
@@ -3957,7 +4604,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>160</v>
       </c>
@@ -3974,7 +4621,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>161</v>
       </c>
@@ -3991,7 +4638,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>162</v>
       </c>
@@ -4008,7 +4655,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>163</v>
       </c>
@@ -4025,7 +4672,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -4042,7 +4689,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>164</v>
       </c>
@@ -4059,7 +4706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>165</v>
       </c>
@@ -4076,7 +4723,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>166</v>
       </c>
@@ -4093,7 +4740,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>167</v>
       </c>
@@ -4110,7 +4757,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>168</v>
       </c>
@@ -4127,7 +4774,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>169</v>
       </c>
@@ -4144,7 +4791,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>170</v>
       </c>
@@ -4161,7 +4808,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>171</v>
       </c>
@@ -4178,7 +4825,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>172</v>
       </c>
@@ -4195,7 +4842,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>144</v>
       </c>
@@ -4212,7 +4859,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>173</v>
       </c>
@@ -4229,7 +4876,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>121</v>
       </c>
@@ -4246,7 +4893,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>174</v>
       </c>
@@ -4263,7 +4910,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>175</v>
       </c>
@@ -4280,7 +4927,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>176</v>
       </c>
@@ -4297,7 +4944,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>177</v>
       </c>
@@ -4314,7 +4961,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>178</v>
       </c>
@@ -4331,7 +4978,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>179</v>
       </c>
@@ -4354,14 +5001,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -4378,7 +5025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>192</v>
       </c>
@@ -4395,7 +5042,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
@@ -4412,7 +5059,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>193</v>
       </c>
@@ -4429,7 +5076,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>194</v>
       </c>
@@ -4446,7 +5093,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>54</v>
       </c>
@@ -4463,7 +5110,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>195</v>
       </c>
@@ -4480,7 +5127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>196</v>
       </c>
@@ -4497,7 +5144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>197</v>
       </c>
@@ -4514,7 +5161,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>198</v>
       </c>
@@ -4531,7 +5178,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>199</v>
       </c>
@@ -4548,7 +5195,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>164</v>
       </c>
@@ -4565,7 +5212,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>59</v>
       </c>
@@ -4582,7 +5229,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>200</v>
       </c>
@@ -4599,7 +5246,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>117</v>
       </c>
@@ -4616,7 +5263,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>201</v>
       </c>
@@ -4633,7 +5280,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>118</v>
       </c>
@@ -4650,7 +5297,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>179</v>
       </c>
@@ -4667,7 +5314,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>202</v>
       </c>
@@ -4684,7 +5331,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>203</v>
       </c>
@@ -4701,7 +5348,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>204</v>
       </c>
@@ -4718,7 +5365,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
@@ -4735,7 +5382,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>205</v>
       </c>
@@ -4752,7 +5399,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>206</v>
       </c>
@@ -4769,7 +5416,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>207</v>
       </c>
@@ -4786,7 +5433,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>208</v>
       </c>
@@ -4803,7 +5450,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>209</v>
       </c>
@@ -4820,7 +5467,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>210</v>
       </c>
@@ -4843,14 +5490,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -4867,7 +5514,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>192</v>
       </c>
@@ -4884,7 +5531,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -4901,7 +5548,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>216</v>
       </c>
@@ -4918,7 +5565,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>217</v>
       </c>
@@ -4935,7 +5582,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>87</v>
       </c>
@@ -4952,7 +5599,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -4969,7 +5616,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>218</v>
       </c>
@@ -4986,7 +5633,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>219</v>
       </c>
@@ -5003,7 +5650,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>92</v>
       </c>
@@ -5020,7 +5667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>220</v>
       </c>
@@ -5037,7 +5684,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>221</v>
       </c>
@@ -5054,7 +5701,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>93</v>
       </c>
@@ -5071,7 +5718,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>94</v>
       </c>
@@ -5088,7 +5735,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>169</v>
       </c>
@@ -5105,7 +5752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>222</v>
       </c>
@@ -5122,7 +5769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>223</v>
       </c>
@@ -5139,7 +5786,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>172</v>
       </c>
@@ -5156,7 +5803,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>224</v>
       </c>
@@ -5173,7 +5820,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>173</v>
       </c>
@@ -5190,7 +5837,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>225</v>
       </c>
@@ -5207,7 +5854,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>98</v>
       </c>
@@ -5224,7 +5871,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>100</v>
       </c>
@@ -5241,7 +5888,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>65</v>
       </c>
@@ -5258,7 +5905,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>178</v>
       </c>
@@ -5275,7 +5922,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>102</v>
       </c>
@@ -5292,7 +5939,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -5309,7 +5956,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>67</v>
       </c>
@@ -5332,14 +5979,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -5356,7 +6003,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>159</v>
       </c>
@@ -5373,7 +6020,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>228</v>
       </c>
@@ -5390,7 +6037,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -5407,7 +6054,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>229</v>
       </c>
@@ -5424,7 +6071,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>161</v>
       </c>
@@ -5441,7 +6088,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>230</v>
       </c>
@@ -5458,7 +6105,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>162</v>
       </c>
@@ -5475,7 +6122,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>231</v>
       </c>
@@ -5492,7 +6139,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>232</v>
       </c>
@@ -5509,7 +6156,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>233</v>
       </c>
@@ -5526,7 +6173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>234</v>
       </c>
@@ -5543,7 +6190,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>235</v>
       </c>
@@ -5560,7 +6207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>236</v>
       </c>
@@ -5577,7 +6224,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>237</v>
       </c>
@@ -5594,7 +6241,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>238</v>
       </c>
@@ -5611,7 +6258,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>64</v>
       </c>
@@ -5628,7 +6275,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>148</v>
       </c>
@@ -5645,7 +6292,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>239</v>
       </c>
@@ -5662,7 +6309,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>240</v>
       </c>
@@ -5679,7 +6326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -5696,7 +6343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>241</v>
       </c>
@@ -5713,7 +6360,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>242</v>
       </c>
@@ -5730,7 +6377,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>125</v>
       </c>
@@ -5747,7 +6394,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
@@ -5764,7 +6411,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>243</v>
       </c>

</xml_diff>